<commit_message>
dev-ds/update-libraries: upgrade tricky client-side libs
bootstrap, react-autosuggest, react-transition-group, reactstrap
</commit_message>
<xml_diff>
--- a/_info/package-update.xlsx
+++ b/_info/package-update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsri/Dev/INQ/netcreate-itest/_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801CC7BD-0EA9-624D-95CE-8C8C7CE8D7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C01F3EF-CA08-FA46-AF96-4F3CC92793C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24000" yWindow="14840" windowWidth="24000" windowHeight="18960" xr2:uid="{5A37D997-27B8-B14B-8590-78FC23DE2F0C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="179">
   <si>
     <t>@babel/core</t>
   </si>
@@ -130,9 +130,15 @@
     <t>react-popper</t>
   </si>
   <si>
+    <t>react-router-config</t>
+  </si>
+  <si>
     <t>react-router-dom</t>
   </si>
   <si>
+    <t>react-transition-group</t>
+  </si>
+  <si>
     <t>reactstrap</t>
   </si>
   <si>
@@ -490,15 +496,9 @@
     <t>react req updated (should be OK)</t>
   </si>
   <si>
-    <t>node 'hashids/cjs' breaking</t>
-  </si>
-  <si>
     <t>possible node esm issues</t>
   </si>
   <si>
-    <t>possible breaking changes</t>
-  </si>
-  <si>
     <t>changelog</t>
   </si>
   <si>
@@ -557,6 +557,21 @@
   </si>
   <si>
     <t>2-client-ben</t>
+  </si>
+  <si>
+    <t>0-ok</t>
+  </si>
+  <si>
+    <t>3-server</t>
+  </si>
+  <si>
+    <t>can't upgrade past 8.1 (brunch?)</t>
+  </si>
+  <si>
+    <t>node 'hashids/cjs' breaking? Worked!</t>
+  </si>
+  <si>
+    <t>4-client</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC6E536-9D6C-1742-8822-815313491C41}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1057,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1056,20 +1071,20 @@
         <v>166</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1078,7 +1093,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1090,19 +1105,19 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1114,19 +1129,19 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1138,7 +1153,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
         <v>172</v>
@@ -1147,70 +1162,76 @@
         <v>172</v>
       </c>
       <c r="G8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>174</v>
+      </c>
       <c r="B10" s="5"/>
       <c r="C10" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G11" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1219,55 +1240,58 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
       <c r="B16" s="5"/>
       <c r="C16" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E16" t="s">
         <v>169</v>
@@ -1280,24 +1304,27 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
       <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G17" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1309,19 +1336,19 @@
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1333,45 +1360,48 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>178</v>
+      </c>
       <c r="B20" s="5"/>
       <c r="C20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1381,19 +1411,19 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G23" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1402,19 +1432,19 @@
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1423,50 +1453,56 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>175</v>
+      </c>
       <c r="B27" s="5"/>
       <c r="C27" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>175</v>
+      </c>
       <c r="B28" s="5"/>
       <c r="C28" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1475,19 +1511,19 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G29" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1496,7 +1532,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -1506,16 +1542,16 @@
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -1527,25 +1563,28 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>175</v>
+      </c>
       <c r="B35" s="5"/>
       <c r="C35" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" t="s">
-        <v>153</v>
+        <v>73</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>176</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>154</v>
@@ -1560,13 +1599,13 @@
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G36" t="s">
         <v>155</v>
@@ -1581,13 +1620,13 @@
         <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G37" t="s">
         <v>155</v>
@@ -1602,13 +1641,13 @@
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G38" t="s">
         <v>156</v>
@@ -1623,16 +1662,16 @@
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G39" t="s">
         <v>157</v>
@@ -1650,13 +1689,13 @@
         <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E40" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G40" t="s">
         <v>156</v>
@@ -1671,7 +1710,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1683,13 +1722,13 @@
         <v>23</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E43" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F43" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G43" t="s">
         <v>160</v>
@@ -1701,16 +1740,16 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D44" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E44" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F44" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G44" t="s">
         <v>160</v>
@@ -1722,7 +1761,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1731,13 +1770,13 @@
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E47" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F47" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G47" t="s">
         <v>161</v>
@@ -1749,13 +1788,13 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E48" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G48" t="s">
         <v>161</v>
@@ -1767,13 +1806,13 @@
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F49" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G49" t="s">
         <v>161</v>
@@ -1782,16 +1821,16 @@
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="5"/>
       <c r="C50" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E50" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F50" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G50" t="s">
         <v>161</v>
@@ -1803,13 +1842,13 @@
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E51" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G51" t="s">
         <v>161</v>
@@ -1821,13 +1860,13 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E52" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F52" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G52" t="s">
         <v>162</v>
@@ -1839,13 +1878,13 @@
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E53" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F53" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
@@ -1854,7 +1893,7 @@
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
@@ -1863,13 +1902,13 @@
         <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E56" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F56" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G56" t="s">
         <v>164</v>
@@ -1881,13 +1920,13 @@
         <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E57" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F57" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G57" t="s">
         <v>164</v>
@@ -1899,13 +1938,13 @@
         <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E58" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F58" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G58" t="s">
         <v>164</v>
@@ -1917,7 +1956,7 @@
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
@@ -1926,13 +1965,13 @@
         <v>24</v>
       </c>
       <c r="D61" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E61" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F61" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G61" t="s">
         <v>160</v>
@@ -1947,7 +1986,7 @@
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
@@ -1955,13 +1994,13 @@
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E64" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F64" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G64" t="s">
         <v>163</v>
@@ -1973,13 +2012,13 @@
         <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E65" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G65" t="s">
         <v>163</v>
@@ -1991,13 +2030,13 @@
         <v>29</v>
       </c>
       <c r="D66" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E66" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F66" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G66" t="s">
         <v>163</v>

</xml_diff>

<commit_message>
dev-ds/update-libraries: update package update xlsx
</commit_message>
<xml_diff>
--- a/_info/package-update.xlsx
+++ b/_info/package-update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsri/Dev/INQ/netcreate-itest/_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE42792-A29B-7743-9153-EFF8BBD2D752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954599E4-1063-0440-B0E7-D035549677D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24000" yWindow="14840" windowWidth="24000" windowHeight="18960" xr2:uid="{5A37D997-27B8-B14B-8590-78FC23DE2F0C}"/>
+    <workbookView xWindow="-24020" yWindow="14840" windowWidth="24000" windowHeight="18960" xr2:uid="{5A37D997-27B8-B14B-8590-78FC23DE2F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC6E536-9D6C-1742-8822-815313491C41}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
dev-ds/update-libraries: purge unused dependencies
core-js, react-is, react-popper
</commit_message>
<xml_diff>
--- a/_info/package-update.xlsx
+++ b/_info/package-update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsri/Dev/INQ/netcreate-itest/_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954599E4-1063-0440-B0E7-D035549677D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ABD260-0270-A540-96B6-CF3B6B979027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24020" yWindow="14840" windowWidth="24000" windowHeight="18960" xr2:uid="{5A37D997-27B8-B14B-8590-78FC23DE2F0C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="183">
   <si>
     <t>@babel/core</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t>require newer build tool</t>
+  </si>
+  <si>
+    <t>6-purge</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC6E536-9D6C-1742-8822-815313491C41}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1846,7 +1849,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B49" s="5"/>
       <c r="C49" s="8" t="s">
         <v>7</v>
@@ -1864,7 +1867,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B50" s="5"/>
       <c r="C50" s="8" t="s">
         <v>38</v>
@@ -1882,7 +1885,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B51" s="5"/>
       <c r="C51" s="9" t="s">
         <v>4</v>
@@ -1900,7 +1903,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B52" s="5"/>
       <c r="C52" s="9" t="s">
         <v>0</v>
@@ -1918,7 +1921,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B53" s="5"/>
       <c r="C53" s="8" t="s">
         <v>3</v>
@@ -1933,16 +1936,16 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="5"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" s="5"/>
       <c r="C56" s="8" t="s">
         <v>12</v>
@@ -1960,7 +1963,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57" s="5"/>
       <c r="C57" s="8" t="s">
         <v>13</v>
@@ -1978,7 +1981,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B58" s="5"/>
       <c r="C58" s="8" t="s">
         <v>14</v>
@@ -1996,16 +1999,16 @@
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" s="5"/>
       <c r="C61" s="2" t="s">
         <v>24</v>
@@ -2026,16 +2029,19 @@
         <v>154</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B62" s="5"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B63" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>182</v>
+      </c>
       <c r="C64" s="9" t="s">
         <v>9</v>
       </c>
@@ -2052,7 +2058,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>182</v>
+      </c>
       <c r="B65" s="5"/>
       <c r="C65" s="9" t="s">
         <v>30</v>
@@ -2070,7 +2079,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>182</v>
+      </c>
       <c r="B66" s="5"/>
       <c r="C66" s="9" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
dev-ds/update-libraries: update gitignore, package-update spreadsheet
</commit_message>
<xml_diff>
--- a/_info/package-update.xlsx
+++ b/_info/package-update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsri/Dev/INQ/netcreate-itest/_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ABD260-0270-A540-96B6-CF3B6B979027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9D7B1B-32F2-5844-B185-BD14BB03F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24020" yWindow="14840" windowWidth="24000" windowHeight="18960" xr2:uid="{5A37D997-27B8-B14B-8590-78FC23DE2F0C}"/>
   </bookViews>
@@ -1062,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC6E536-9D6C-1742-8822-815313491C41}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>

</xml_diff>